<commit_message>
created a bar char for visualisation
</commit_message>
<xml_diff>
--- a/expenditure.xlsx
+++ b/expenditure.xlsx
@@ -14,13 +14,13 @@
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
   <si>
     <t>JANUARY</t>
   </si>
@@ -40,25 +40,7 @@
     <t>JUNE</t>
   </si>
   <si>
-    <t>JULY</t>
-  </si>
-  <si>
-    <t>AUGUST</t>
-  </si>
-  <si>
-    <t>SEPTEMBER</t>
-  </si>
-  <si>
     <t>ITEM CATEGORY</t>
-  </si>
-  <si>
-    <t>OCTOBER</t>
-  </si>
-  <si>
-    <t>NOVEMBER</t>
-  </si>
-  <si>
-    <t>DECEMBER</t>
   </si>
   <si>
     <t>BEAUTY</t>
@@ -672,7 +654,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K5:Q46" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1204,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1225,10 +1207,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1248,31 +1230,13 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>3000</v>
@@ -1295,10 +1259,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>2000</v>
@@ -1321,10 +1285,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>500</v>
@@ -1347,10 +1311,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>300</v>
@@ -1371,33 +1335,33 @@
         <v>200</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" t="s">
         <v>55</v>
-      </c>
-      <c r="L5" t="s">
-        <v>54</v>
-      </c>
-      <c r="M5" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" t="s">
-        <v>59</v>
-      </c>
-      <c r="P5" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>2000</v>
@@ -1418,7 +1382,7 @@
         <v>1500</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L6" s="1">
         <v>8000</v>
@@ -1441,10 +1405,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>800</v>
@@ -1465,7 +1429,7 @@
         <v>500</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
@@ -1488,10 +1452,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>700</v>
@@ -1512,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L8" s="1">
         <v>3000</v>
@@ -1535,10 +1499,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>500</v>
@@ -1559,7 +1523,7 @@
         <v>200</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L9" s="1">
         <v>3000</v>
@@ -1582,10 +1546,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>400</v>
@@ -1606,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -1629,10 +1593,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>800</v>
@@ -1653,7 +1617,7 @@
         <v>600</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L11" s="1">
         <v>500</v>
@@ -1676,10 +1640,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>1000</v>
@@ -1700,7 +1664,7 @@
         <v>150</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L12" s="1">
         <v>1500</v>
@@ -1723,10 +1687,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>600</v>
@@ -1747,7 +1711,7 @@
         <v>500</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L13" s="1">
         <v>2000</v>
@@ -1770,10 +1734,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>4000</v>
@@ -1794,7 +1758,7 @@
         <v>1000</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L14" s="1">
         <v>2000</v>
@@ -1817,10 +1781,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>1500</v>
@@ -1841,7 +1805,7 @@
         <v>1600</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L15" s="1">
         <v>4100</v>
@@ -1864,10 +1828,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>6000</v>
@@ -1888,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L16" s="1">
         <v>600</v>
@@ -1911,10 +1875,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C17">
         <v>700</v>
@@ -1935,7 +1899,7 @@
         <v>700</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L17" s="1">
         <v>3500</v>
@@ -1958,10 +1922,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>1200</v>
@@ -1982,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L18" s="1">
         <v>10600</v>
@@ -2005,10 +1969,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>2000</v>
@@ -2029,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="L19" s="1">
         <v>300</v>
@@ -2052,10 +2016,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1000</v>
@@ -2076,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="L20" s="1">
         <v>1000</v>
@@ -2099,10 +2063,10 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>2500</v>
@@ -2123,7 +2087,7 @@
         <v>3000</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L21" s="1">
         <v>3000</v>
@@ -2146,10 +2110,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>3500</v>
@@ -2170,7 +2134,7 @@
         <v>3500</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L22" s="1">
         <v>700</v>
@@ -2193,10 +2157,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>600</v>
@@ -2217,7 +2181,7 @@
         <v>500</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L23" s="1">
         <v>800</v>
@@ -2240,10 +2204,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C24">
         <v>10000</v>
@@ -2264,7 +2228,7 @@
         <v>10000</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L24" s="1">
         <v>800</v>
@@ -2287,10 +2251,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>500</v>
@@ -2311,7 +2275,7 @@
         <v>300</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L25" s="1">
         <v>600</v>
@@ -2334,10 +2298,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <v>500</v>
@@ -2358,7 +2322,7 @@
         <v>300</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="L26" s="1">
         <v>500</v>
@@ -2381,31 +2345,31 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>3000</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>3000</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C27">
-        <v>3000</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>3000</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="L27" s="1">
         <v>400</v>
@@ -2428,10 +2392,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C28">
         <v>500</v>
@@ -2452,7 +2416,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L28" s="1">
         <v>500</v>
@@ -2475,10 +2439,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C29">
         <v>1500</v>
@@ -2499,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L29" s="1">
         <v>2000</v>
@@ -2522,10 +2486,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C30">
         <v>3000</v>
@@ -2546,7 +2510,7 @@
         <v>3000</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="L30" s="1">
         <v>11500</v>
@@ -2569,10 +2533,10 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2593,7 +2557,7 @@
         <v>1000</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L31" s="1">
         <v>500</v>
@@ -2616,10 +2580,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <v>500</v>
@@ -2640,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="L32" s="1">
         <v>10000</v>
@@ -2663,10 +2627,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2687,7 +2651,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L33" s="1">
         <v>500</v>
@@ -2710,7 +2674,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K34" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L34" s="1">
         <v>500</v>
@@ -2733,7 +2697,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K35" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L35" s="1">
         <v>3900</v>
@@ -2756,7 +2720,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K36" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L36" s="1">
         <v>2000</v>
@@ -2779,7 +2743,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K37" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L37" s="1">
         <v>700</v>
@@ -2802,7 +2766,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K38" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="L38" s="1">
         <v>1200</v>
@@ -2825,7 +2789,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K39" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L39" s="1">
         <v>3500</v>
@@ -2848,7 +2812,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K40" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L40" s="1">
         <v>2500</v>
@@ -2871,7 +2835,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K41" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="L41" s="1">
         <v>1000</v>
@@ -2894,7 +2858,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K42" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L42" s="1">
         <v>11500</v>
@@ -2917,7 +2881,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K43" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L43" s="1">
         <v>1500</v>
@@ -2940,7 +2904,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K44" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="L44" s="1">
         <v>4000</v>
@@ -2963,7 +2927,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K45" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L45" s="1">
         <v>6000</v>
@@ -2986,7 +2950,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K46" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L46" s="1">
         <v>55100</v>

</xml_diff>